<commit_message>
Combined feature agent result
</commit_message>
<xml_diff>
--- a/data/results/raw_sentiment_features/untrained_testing.xlsx
+++ b/data/results/raw_sentiment_features/untrained_testing.xlsx
@@ -478,34 +478,34 @@
         <v>1</v>
       </c>
       <c r="C2" t="n">
-        <v>1692207.448135082</v>
+        <v>1692744.504728717</v>
       </c>
       <c r="D2" t="n">
-        <v>1691218.263525296</v>
+        <v>1691864.841200692</v>
       </c>
       <c r="E2" t="n">
-        <v>1692185.131420611</v>
+        <v>1692749.092345976</v>
       </c>
       <c r="F2" t="n">
-        <v>1693021.223606169</v>
+        <v>1691618.081491214</v>
       </c>
       <c r="G2" t="n">
-        <v>1689840.35509893</v>
+        <v>1691967.686920107</v>
       </c>
       <c r="H2" t="n">
-        <v>1692560.919070486</v>
+        <v>1693300.129814962</v>
       </c>
       <c r="I2" t="n">
-        <v>1693136.81249047</v>
+        <v>1691570.564286089</v>
       </c>
       <c r="J2" t="n">
-        <v>1692470.946129007</v>
+        <v>1692426.165228999</v>
       </c>
       <c r="K2" t="n">
-        <v>1693690.274146855</v>
+        <v>1692237.904945076</v>
       </c>
       <c r="L2" t="n">
-        <v>1692137.75388348</v>
+        <v>1692090.165077803</v>
       </c>
     </row>
   </sheetData>

</xml_diff>